<commit_message>
Expand Key Metrics to 8 items with Net Profit Margin
</commit_message>
<xml_diff>
--- a/data/TIX.xlsx
+++ b/data/TIX.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="352">
   <si>
     <t>Liên Hệ</t>
   </si>
@@ -73,7 +73,7 @@
     <t>Ngày xuất</t>
   </si>
   <si>
-    <t>21/12/2025</t>
+    <t>23/12/2025</t>
   </si>
   <si>
     <t>TIX</t>
@@ -2168,7 +2168,7 @@
         <v>5.73890987077E11</v>
       </c>
       <c r="AS12" s="13" t="n">
-        <v>6.05095580025E11</v>
+        <v>5.96427093955E11</v>
       </c>
     </row>
     <row r="13">
@@ -3240,7 +3240,7 @@
         <v>3.6299016938E10</v>
       </c>
       <c r="AS20" s="13" t="n">
-        <v>6.2376667977E10</v>
+        <v>5.3708181907E10</v>
       </c>
     </row>
     <row r="21">
@@ -3374,7 +3374,7 @@
         <v>2.1765078258E10</v>
       </c>
       <c r="AS21" s="13" t="n">
-        <v>2.2617093632E10</v>
+        <v>1.3988607562E10</v>
       </c>
     </row>
     <row r="22">
@@ -4044,7 +4044,7 @@
         <v>1.3679027464E10</v>
       </c>
       <c r="AS26" s="13" t="n">
-        <v>4.1255800431E10</v>
+        <v>4.1215800431E10</v>
       </c>
     </row>
     <row r="27">
@@ -5652,7 +5652,7 @@
         <v>6.41224444768E11</v>
       </c>
       <c r="AS38" s="13" t="n">
-        <v>6.19948916699E11</v>
+        <v>6.30020259743E11</v>
       </c>
     </row>
     <row r="39">
@@ -5786,7 +5786,7 @@
         <v>7.284723529E9</v>
       </c>
       <c r="AS39" s="13" t="n">
-        <v>7.284723529E9</v>
+        <v>1.5953209599E10</v>
       </c>
     </row>
     <row r="40">
@@ -5920,7 +5920,7 @@
         <v>0.0</v>
       </c>
       <c r="AS40" s="13" t="n">
-        <v>0.0</v>
+        <v>8.62848607E9</v>
       </c>
     </row>
     <row r="41">
@@ -6590,7 +6590,7 @@
         <v>5.719707E9</v>
       </c>
       <c r="AS45" s="13" t="n">
-        <v>5.719707E9</v>
+        <v>5.759707E9</v>
       </c>
     </row>
     <row r="46">
@@ -9136,7 +9136,7 @@
         <v>1.53971020666E11</v>
       </c>
       <c r="AS64" s="13" t="n">
-        <v>1.39254689158E11</v>
+        <v>1.40657546132E11</v>
       </c>
     </row>
     <row r="65">
@@ -9672,7 +9672,7 @@
         <v>-1.6214868462E10</v>
       </c>
       <c r="AS68" s="13" t="n">
-        <v>-8.02E9</v>
+        <v>-6.617143026E9</v>
       </c>
     </row>
     <row r="69">
@@ -10878,7 +10878,7 @@
         <v>1.215115431845E12</v>
       </c>
       <c r="AS77" s="13" t="n">
-        <v>1.225044496724E12</v>
+        <v>1.226447353698E12</v>
       </c>
     </row>
     <row r="78">
@@ -11012,7 +11012,7 @@
         <v>3.83549334166E11</v>
       </c>
       <c r="AS78" s="13" t="n">
-        <v>3.71178013147E11</v>
+        <v>3.71458584542E11</v>
       </c>
     </row>
     <row r="79">
@@ -11146,7 +11146,7 @@
         <v>1.25743471504E11</v>
       </c>
       <c r="AS79" s="13" t="n">
-        <v>1.17636706676E11</v>
+        <v>1.17917278071E11</v>
       </c>
     </row>
     <row r="80">
@@ -11548,7 +11548,7 @@
         <v>3.8401307905E10</v>
       </c>
       <c r="AS82" s="13" t="n">
-        <v>2.4780447193E10</v>
+        <v>2.5061018588E10</v>
       </c>
     </row>
     <row r="83">
@@ -15080,7 +15080,7 @@
         <v>8.31566097679E11</v>
       </c>
       <c r="AS109" s="13" t="n">
-        <v>8.53866483577E11</v>
+        <v>8.54988769156E11</v>
       </c>
     </row>
     <row r="110">
@@ -15214,7 +15214,7 @@
         <v>8.31566097679E11</v>
       </c>
       <c r="AS110" s="13" t="n">
-        <v>8.53866483577E11</v>
+        <v>8.54988769156E11</v>
       </c>
     </row>
     <row r="111">
@@ -17090,7 +17090,7 @@
         <v>2.09524886541E11</v>
       </c>
       <c r="AS124" s="13" t="n">
-        <v>2.31825272439E11</v>
+        <v>2.32947558018E11</v>
       </c>
     </row>
     <row r="125">
@@ -17358,7 +17358,7 @@
         <v>5.5649133175E10</v>
       </c>
       <c r="AS126" s="13" t="n">
-        <v>7.7949519073E10</v>
+        <v>7.9071804652E10</v>
       </c>
     </row>
     <row r="127">
@@ -18296,7 +18296,7 @@
         <v>1.215115431845E12</v>
       </c>
       <c r="AS133" s="13" t="n">
-        <v>1.225044496724E12</v>
+        <v>1.226447353698E12</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
@@ -19518,7 +19518,7 @@
         <v>-139321.0</v>
       </c>
       <c r="AS18" s="17" t="n">
-        <v>-1.2859378473E10</v>
+        <v>-1.1456521499E10</v>
       </c>
     </row>
     <row r="19">
@@ -20188,7 +20188,7 @@
         <v>4.8200794336E10</v>
       </c>
       <c r="AS23" s="17" t="n">
-        <v>2.768739513E10</v>
+        <v>2.9090252104E10</v>
       </c>
     </row>
     <row r="24">
@@ -20858,7 +20858,7 @@
         <v>4.8069493341E10</v>
       </c>
       <c r="AS28" s="17" t="n">
-        <v>2.8398615388E10</v>
+        <v>2.9801472362E10</v>
       </c>
     </row>
     <row r="29">
@@ -20992,7 +20992,7 @@
         <v>-9.154260679E9</v>
       </c>
       <c r="AS29" s="17" t="n">
-        <v>-6.09822949E9</v>
+        <v>-6.378800885E9</v>
       </c>
     </row>
     <row r="30">
@@ -21126,7 +21126,7 @@
         <v>-9.154260679E9</v>
       </c>
       <c r="AS30" s="17" t="n">
-        <v>-5.991277796E9</v>
+        <v>-6.271849191E9</v>
       </c>
     </row>
     <row r="31">
@@ -21394,7 +21394,7 @@
         <v>3.8915232662E10</v>
       </c>
       <c r="AS32" s="17" t="n">
-        <v>2.2300385898E10</v>
+        <v>2.3422671477E10</v>
       </c>
     </row>
     <row r="33">
@@ -21662,7 +21662,7 @@
         <v>3.8915232662E10</v>
       </c>
       <c r="AS34" s="17" t="n">
-        <v>2.2300385898E10</v>
+        <v>2.3422671477E10</v>
       </c>
     </row>
     <row r="35">
@@ -21796,7 +21796,7 @@
         <v>1134.0</v>
       </c>
       <c r="AS35" s="17" t="n">
-        <v>647.0</v>
+        <v>588.0</v>
       </c>
     </row>
     <row r="36">
@@ -21930,7 +21930,7 @@
         <v>1134.0</v>
       </c>
       <c r="AS36" s="17" t="n">
-        <v>647.0</v>
+        <v>588.0</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -23688,7 +23688,7 @@
         <v>5.0618009451E10</v>
       </c>
       <c r="AS22" s="21" t="n">
-        <v>2.7778720401E10</v>
+        <v>2.7818446076E10</v>
       </c>
     </row>
     <row r="23">
@@ -25162,7 +25162,7 @@
         <v>-1.5956756702E10</v>
       </c>
       <c r="AS33" s="21" t="n">
-        <v>-2.0947019418E10</v>
+        <v>-2.0986745093E10</v>
       </c>
     </row>
     <row r="34">
@@ -26100,7 +26100,7 @@
         <v>1.2446322742E10</v>
       </c>
       <c r="AS40" s="21" t="n">
-        <v>6.814380582E9</v>
+        <v>6.774654907E9</v>
       </c>
     </row>
     <row r="41">
@@ -27763,7 +27763,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ACDB1F9-64B2-F64B-91A6-B0AAFF7D49C4}">
-  <dimension ref="A1:V176"/>
+  <dimension ref="A1:Z176"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -27793,6 +27793,10 @@
     <col min="20" max="20" width="16.7890625" customWidth="true" bestFit="true"/>
     <col min="21" max="21" width="16.7890625" customWidth="true" bestFit="true"/>
     <col min="22" max="22" width="16.7890625" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.7890625" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="16.7890625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="16.7890625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="16.7890625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -27902,6 +27906,18 @@
       <c r="V11" s="6" t="s">
         <v>46</v>
       </c>
+      <c r="W11" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="X11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y11" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z11" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="28" t="s">
@@ -27967,6 +27983,18 @@
       <c r="V12" s="25" t="n">
         <v>4.7437268487E10</v>
       </c>
+      <c r="W12" s="25" t="n">
+        <v>5.5726787651E10</v>
+      </c>
+      <c r="X12" s="25" t="n">
+        <v>7.1167365376E10</v>
+      </c>
+      <c r="Y12" s="25" t="n">
+        <v>5.3523274125E10</v>
+      </c>
+      <c r="Z12" s="25" t="n">
+        <v>6.0204915141E10</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="26" t="s">
@@ -28032,6 +28060,18 @@
       <c r="V13" s="25" t="n">
         <v>1.0733869E9</v>
       </c>
+      <c r="W13" s="25" t="n">
+        <v>1.443197408E9</v>
+      </c>
+      <c r="X13" s="25" t="n">
+        <v>1.165878284E9</v>
+      </c>
+      <c r="Y13" s="25" t="n">
+        <v>1.257149161E9</v>
+      </c>
+      <c r="Z13" s="25" t="n">
+        <v>1.4429885E9</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="26" t="s">
@@ -28097,6 +28137,18 @@
       <c r="V14" s="25" t="n">
         <v>4.6363881587E10</v>
       </c>
+      <c r="W14" s="25" t="n">
+        <v>5.4283590243E10</v>
+      </c>
+      <c r="X14" s="25" t="n">
+        <v>5.5001487092E10</v>
+      </c>
+      <c r="Y14" s="25" t="n">
+        <v>5.2266124964E10</v>
+      </c>
+      <c r="Z14" s="25" t="n">
+        <v>4.8761926641E10</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="26" t="s">
@@ -28162,6 +28214,18 @@
       <c r="V15" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W15" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X15" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y15" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z15" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="26" t="s">
@@ -28227,6 +28291,18 @@
       <c r="V16" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W16" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X16" s="25" t="n">
+        <v>1.5E10</v>
+      </c>
+      <c r="Y16" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z16" s="25" t="n">
+        <v>1.0E10</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="26" t="s">
@@ -28292,6 +28368,18 @@
       <c r="V17" s="25" t="n">
         <v>4.5503263555E11</v>
       </c>
+      <c r="W17" s="25" t="n">
+        <v>4.36748358617E11</v>
+      </c>
+      <c r="X17" s="25" t="n">
+        <v>4.4794897125E11</v>
+      </c>
+      <c r="Y17" s="25" t="n">
+        <v>4.7524897125E11</v>
+      </c>
+      <c r="Z17" s="25" t="n">
+        <v>4.781093579E11</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="28" t="s">
@@ -28357,6 +28445,18 @@
       <c r="V18" s="25" t="n">
         <v>8.017244484E9</v>
       </c>
+      <c r="W18" s="25" t="n">
+        <v>6.696042576E9</v>
+      </c>
+      <c r="X18" s="25" t="n">
+        <v>4.55378025E9</v>
+      </c>
+      <c r="Y18" s="25" t="n">
+        <v>4.55378025E9</v>
+      </c>
+      <c r="Z18" s="25" t="n">
+        <v>1.43795571E9</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="26" t="s">
@@ -28422,6 +28522,18 @@
       <c r="V19" s="25" t="n">
         <v>4.471261863E11</v>
       </c>
+      <c r="W19" s="25" t="n">
+        <v>4.301261863E11</v>
+      </c>
+      <c r="X19" s="25" t="n">
+        <v>4.434E11</v>
+      </c>
+      <c r="Y19" s="25" t="n">
+        <v>4.707E11</v>
+      </c>
+      <c r="Z19" s="25" t="n">
+        <v>4.767E11</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="26" t="s">
@@ -28487,6 +28599,18 @@
       <c r="V20" s="25" t="n">
         <v>4.471261863E11</v>
       </c>
+      <c r="W20" s="25" t="n">
+        <v>4.301261863E11</v>
+      </c>
+      <c r="X20" s="25" t="n">
+        <v>4.434E11</v>
+      </c>
+      <c r="Y20" s="25" t="n">
+        <v>4.707E11</v>
+      </c>
+      <c r="Z20" s="25" t="n">
+        <v>4.767E11</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="26" t="s">
@@ -28552,6 +28676,18 @@
       <c r="V21" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W21" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X21" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y21" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z21" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="26" t="s">
@@ -28617,6 +28753,18 @@
       <c r="V22" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W22" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X22" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y22" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z22" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="26" t="s">
@@ -28682,6 +28830,18 @@
       <c r="V23" s="25" t="n">
         <v>-1.10795234E8</v>
       </c>
+      <c r="W23" s="25" t="n">
+        <v>-7.3870259E7</v>
+      </c>
+      <c r="X23" s="25" t="n">
+        <v>-4809000.0</v>
+      </c>
+      <c r="Y23" s="25" t="n">
+        <v>-4809000.0</v>
+      </c>
+      <c r="Z23" s="25" t="n">
+        <v>-2.859781E7</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="28" t="s">
@@ -28747,6 +28907,18 @@
       <c r="V24" s="25" t="n">
         <v>1.131730955E10</v>
       </c>
+      <c r="W24" s="25" t="n">
+        <v>1.1630633203E10</v>
+      </c>
+      <c r="X24" s="25" t="n">
+        <v>1.8877714771E10</v>
+      </c>
+      <c r="Y24" s="25" t="n">
+        <v>1.3679027464E10</v>
+      </c>
+      <c r="Z24" s="25" t="n">
+        <v>4.1215800431E10</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="26" t="s">
@@ -28812,6 +28984,18 @@
       <c r="V25" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W25" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X25" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y25" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z25" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="26" t="s">
@@ -28877,6 +29061,18 @@
       <c r="V26" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W26" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X26" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y26" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z26" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="26" t="s">
@@ -28942,6 +29138,18 @@
       <c r="V27" s="25" t="n">
         <v>5000000.0</v>
       </c>
+      <c r="W27" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X27" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y27" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z27" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="26" t="s">
@@ -29007,6 +29215,18 @@
       <c r="V28" s="25" t="n">
         <v>1.131230955E10</v>
       </c>
+      <c r="W28" s="25" t="n">
+        <v>1.1630633203E10</v>
+      </c>
+      <c r="X28" s="25" t="n">
+        <v>1.8877714771E10</v>
+      </c>
+      <c r="Y28" s="25" t="n">
+        <v>1.3679027464E10</v>
+      </c>
+      <c r="Z28" s="25" t="n">
+        <v>4.1215800431E10</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="28" t="s">
@@ -29072,6 +29292,18 @@
       <c r="V29" s="25" t="n">
         <v>6.765E7</v>
       </c>
+      <c r="W29" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X29" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y29" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z29" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="26" t="s">
@@ -29137,6 +29369,18 @@
       <c r="V30" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W30" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X30" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y30" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z30" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="26" t="s">
@@ -29202,6 +29446,18 @@
       <c r="V31" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W31" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X31" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y31" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z31" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="26" t="s">
@@ -29267,6 +29523,18 @@
       <c r="V32" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W32" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X32" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y32" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z32" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="26" t="s">
@@ -29332,6 +29600,18 @@
       <c r="V33" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W33" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X33" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y33" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z33" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="26" t="s">
@@ -29397,6 +29677,18 @@
       <c r="V34" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W34" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X34" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y34" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z34" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="26" t="s">
@@ -29462,6 +29754,18 @@
       <c r="V35" s="25" t="n">
         <v>6.765E7</v>
       </c>
+      <c r="W35" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X35" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y35" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z35" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="26" t="s">
@@ -29527,6 +29831,18 @@
       <c r="V36" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W36" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X36" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y36" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z36" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="26" t="s">
@@ -29592,6 +29908,18 @@
       <c r="V37" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W37" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X37" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y37" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z37" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="26" t="s">
@@ -29657,6 +29985,18 @@
       <c r="V38" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W38" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X38" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y38" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z38" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="28" t="s">
@@ -29722,6 +30062,18 @@
       <c r="V39" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W39" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X39" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y39" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z39" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="26" t="s">
@@ -29787,6 +30139,18 @@
       <c r="V40" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W40" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X40" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y40" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z40" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="26" t="s">
@@ -29852,6 +30216,18 @@
       <c r="V41" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W41" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X41" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y41" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z41" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="26" t="s">
@@ -29917,6 +30293,18 @@
       <c r="V42" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W42" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X42" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y42" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z42" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="26" t="s">
@@ -29982,6 +30370,18 @@
       <c r="V43" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W43" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X43" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y43" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z43" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="28" t="s">
@@ -30047,6 +30447,18 @@
       <c r="V44" s="25" t="n">
         <v>5.719707E9</v>
       </c>
+      <c r="W44" s="25" t="n">
+        <v>5.719707E9</v>
+      </c>
+      <c r="X44" s="25" t="n">
+        <v>5.719707E9</v>
+      </c>
+      <c r="Y44" s="25" t="n">
+        <v>5.719707E9</v>
+      </c>
+      <c r="Z44" s="25" t="n">
+        <v>5.759707E9</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="26" t="s">
@@ -30112,6 +30524,18 @@
       <c r="V45" s="25" t="n">
         <v>5.719707E9</v>
       </c>
+      <c r="W45" s="25" t="n">
+        <v>5.719707E9</v>
+      </c>
+      <c r="X45" s="25" t="n">
+        <v>5.719707E9</v>
+      </c>
+      <c r="Y45" s="25" t="n">
+        <v>5.719707E9</v>
+      </c>
+      <c r="Z45" s="25" t="n">
+        <v>5.759707E9</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="26" t="s">
@@ -30177,6 +30601,18 @@
       <c r="V46" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W46" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X46" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y46" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z46" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="26" t="s">
@@ -30242,6 +30678,18 @@
       <c r="V47" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W47" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X47" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y47" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z47" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="26" t="s">
@@ -30307,6 +30755,18 @@
       <c r="V48" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W48" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X48" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y48" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z48" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="28" t="s">
@@ -30372,6 +30832,18 @@
       <c r="V49" s="25" t="n">
         <v>1.78387542785E11</v>
       </c>
+      <c r="W49" s="25" t="n">
+        <v>1.79055146245E11</v>
+      </c>
+      <c r="X49" s="25" t="n">
+        <v>1.79055146245E11</v>
+      </c>
+      <c r="Y49" s="25" t="n">
+        <v>1.81279346245E11</v>
+      </c>
+      <c r="Z49" s="25" t="n">
+        <v>1.81318896245E11</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="26" t="s">
@@ -30437,6 +30909,18 @@
       <c r="V50" s="25" t="n">
         <v>1.5477227794E11</v>
       </c>
+      <c r="W50" s="25" t="n">
+        <v>1.78387542785E11</v>
+      </c>
+      <c r="X50" s="25" t="n">
+        <v>1.78387542785E11</v>
+      </c>
+      <c r="Y50" s="25" t="n">
+        <v>1.78387542785E11</v>
+      </c>
+      <c r="Z50" s="25" t="n">
+        <v>1.78387542785E11</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="26" t="s">
@@ -30502,6 +30986,18 @@
       <c r="V51" s="25" t="n">
         <v>2.4893783027E10</v>
       </c>
+      <c r="W51" s="25" t="n">
+        <v>6.6760346E8</v>
+      </c>
+      <c r="X51" s="25" t="n">
+        <v>6.6760346E8</v>
+      </c>
+      <c r="Y51" s="25" t="n">
+        <v>2.89180346E9</v>
+      </c>
+      <c r="Z51" s="25" t="n">
+        <v>2.93135346E9</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="26" t="s">
@@ -30567,6 +31063,18 @@
       <c r="V52" s="25" t="n">
         <v>-1.278518182E9</v>
       </c>
+      <c r="W52" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X52" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y52" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z52" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="28" t="s">
@@ -30632,6 +31140,18 @@
       <c r="V53" s="25" t="n">
         <v>1.43737951498E11</v>
       </c>
+      <c r="W53" s="25" t="n">
+        <v>1.45331675409E11</v>
+      </c>
+      <c r="X53" s="25" t="n">
+        <v>1.46928070164E11</v>
+      </c>
+      <c r="Y53" s="25" t="n">
+        <v>1.48567314649E11</v>
+      </c>
+      <c r="Z53" s="25" t="n">
+        <v>1.50257483013E11</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="26" t="s">
@@ -30697,6 +31217,18 @@
       <c r="V54" s="25" t="n">
         <v>1.39867290844E11</v>
       </c>
+      <c r="W54" s="25" t="n">
+        <v>1.43737951498E11</v>
+      </c>
+      <c r="X54" s="25" t="n">
+        <v>1.43737951498E11</v>
+      </c>
+      <c r="Y54" s="25" t="n">
+        <v>1.43737951498E11</v>
+      </c>
+      <c r="Z54" s="25" t="n">
+        <v>1.43737951498E11</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="26" t="s">
@@ -30762,6 +31294,18 @@
       <c r="V55" s="25" t="n">
         <v>5.149178836E9</v>
       </c>
+      <c r="W55" s="25" t="n">
+        <v>1.593723911E9</v>
+      </c>
+      <c r="X55" s="25" t="n">
+        <v>3.190118666E9</v>
+      </c>
+      <c r="Y55" s="25" t="n">
+        <v>4.829363151E9</v>
+      </c>
+      <c r="Z55" s="25" t="n">
+        <v>6.519531515E9</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="26" t="s">
@@ -30827,6 +31371,18 @@
       <c r="V56" s="25" t="n">
         <v>-1.278518182E9</v>
       </c>
+      <c r="W56" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X56" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y56" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z56" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="28" t="s">
@@ -30892,6 +31448,18 @@
       <c r="V57" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W57" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X57" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y57" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z57" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="26" t="s">
@@ -30957,6 +31525,18 @@
       <c r="V58" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W58" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X58" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y58" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z58" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="26" t="s">
@@ -31022,6 +31602,18 @@
       <c r="V59" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W59" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X59" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y59" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z59" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="26" t="s">
@@ -31087,6 +31679,18 @@
       <c r="V60" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W60" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X60" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y60" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z60" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="28" t="s">
@@ -31152,6 +31756,18 @@
       <c r="V61" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W61" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X61" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y61" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z61" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="26" t="s">
@@ -31217,6 +31833,18 @@
       <c r="V62" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W62" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X62" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y62" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z62" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="26" t="s">
@@ -31282,6 +31910,18 @@
       <c r="V63" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W63" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X63" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y63" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z63" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="26" t="s">
@@ -31347,6 +31987,18 @@
       <c r="V64" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W64" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X64" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y64" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z64" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="28" t="s">
@@ -31412,6 +32064,18 @@
       <c r="V65" s="25" t="n">
         <v>4.45E8</v>
       </c>
+      <c r="W65" s="25" t="n">
+        <v>4.45E8</v>
+      </c>
+      <c r="X65" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y65" s="25" t="n">
+        <v>4.45E8</v>
+      </c>
+      <c r="Z65" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="26" t="s">
@@ -31477,6 +32141,18 @@
       <c r="V66" s="25" t="n">
         <v>4.45E8</v>
       </c>
+      <c r="W66" s="25" t="n">
+        <v>4.45E8</v>
+      </c>
+      <c r="X66" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y66" s="25" t="n">
+        <v>4.45E8</v>
+      </c>
+      <c r="Z66" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="26" t="s">
@@ -31542,6 +32218,18 @@
       <c r="V67" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W67" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X67" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y67" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z67" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="26" t="s">
@@ -31607,6 +32295,18 @@
       <c r="V68" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W68" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X68" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y68" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z68" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="28" t="s">
@@ -31672,6 +32372,18 @@
       <c r="V69" s="25" t="n">
         <v>4.45E8</v>
       </c>
+      <c r="W69" s="25" t="n">
+        <v>4.45E8</v>
+      </c>
+      <c r="X69" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y69" s="25" t="n">
+        <v>4.45E8</v>
+      </c>
+      <c r="Z69" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="26" t="s">
@@ -31737,6 +32449,18 @@
       <c r="V70" s="25" t="n">
         <v>4.42E8</v>
       </c>
+      <c r="W70" s="25" t="n">
+        <v>4.45E8</v>
+      </c>
+      <c r="X70" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y70" s="25" t="n">
+        <v>4.45E8</v>
+      </c>
+      <c r="Z70" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="26" t="s">
@@ -31802,6 +32526,18 @@
       <c r="V71" s="25" t="n">
         <v>3000000.0</v>
       </c>
+      <c r="W71" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X71" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y71" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z71" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="26" t="s">
@@ -31867,6 +32603,18 @@
       <c r="V72" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W72" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X72" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y72" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z72" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="28" t="s">
@@ -31932,6 +32680,18 @@
       <c r="V73" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W73" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X73" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y73" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z73" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="26" t="s">
@@ -31997,6 +32757,18 @@
       <c r="V74" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W74" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X74" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y74" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z74" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="26" t="s">
@@ -32062,6 +32834,18 @@
       <c r="V75" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W75" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X75" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y75" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z75" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="26" t="s">
@@ -32127,6 +32911,18 @@
       <c r="V76" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W76" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X76" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y76" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z76" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="26" t="s">
@@ -32192,6 +32988,18 @@
       <c r="V77" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W77" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X77" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y77" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z77" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="26" t="s">
@@ -32257,6 +33065,18 @@
       <c r="V78" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W78" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X78" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y78" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z78" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="28" t="s">
@@ -32322,6 +33142,18 @@
       <c r="V79" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W79" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X79" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y79" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z79" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="26" t="s">
@@ -32387,6 +33219,18 @@
       <c r="V80" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W80" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X80" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y80" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z80" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="26" t="s">
@@ -32452,6 +33296,18 @@
       <c r="V81" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W81" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X81" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y81" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z81" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="28" t="s">
@@ -32517,6 +33373,18 @@
       <c r="V82" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W82" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X82" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y82" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z82" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="26" t="s">
@@ -32582,6 +33450,18 @@
       <c r="V83" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W83" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X83" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y83" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z83" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="26" t="s">
@@ -32647,6 +33527,18 @@
       <c r="V84" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W84" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X84" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y84" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z84" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="26" t="s">
@@ -32712,6 +33604,18 @@
       <c r="V85" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W85" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X85" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y85" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z85" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="28" t="s">
@@ -32777,6 +33681,18 @@
       <c r="V86" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W86" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X86" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y86" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z86" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="26" t="s">
@@ -32842,6 +33758,18 @@
       <c r="V87" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W87" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X87" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y87" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z87" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="26" t="s">
@@ -32907,6 +33835,18 @@
       <c r="V88" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W88" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X88" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y88" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z88" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="26" t="s">
@@ -32972,6 +33912,18 @@
       <c r="V89" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W89" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X89" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y89" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z89" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="28" t="s">
@@ -33037,6 +33989,18 @@
       <c r="V90" s="25" t="n">
         <v>1.4843706132E10</v>
       </c>
+      <c r="W90" s="25" t="n">
+        <v>3.201803551E9</v>
+      </c>
+      <c r="X90" s="25" t="n">
+        <v>4.261285758E9</v>
+      </c>
+      <c r="Y90" s="25" t="n">
+        <v>3.8401307905E10</v>
+      </c>
+      <c r="Z90" s="25" t="n">
+        <v>2.5061018588E10</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="26" t="s">
@@ -33102,6 +34066,18 @@
       <c r="V91" s="25" t="n">
         <v>5.970379122E9</v>
       </c>
+      <c r="W91" s="25" t="n">
+        <v>1.401730524E9</v>
+      </c>
+      <c r="X91" s="25" t="n">
+        <v>1.466218183E9</v>
+      </c>
+      <c r="Y91" s="25" t="n">
+        <v>8.094197422E9</v>
+      </c>
+      <c r="Z91" s="25" t="n">
+        <v>8.177815756E9</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="26" t="s">
@@ -33167,6 +34143,18 @@
       <c r="V92" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W92" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X92" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y92" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z92" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="26" t="s">
@@ -33232,6 +34220,18 @@
       <c r="V93" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W93" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X93" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y93" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z93" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="26" t="s">
@@ -33297,6 +34297,18 @@
       <c r="V94" s="25" t="n">
         <v>2.180842234E9</v>
       </c>
+      <c r="W94" s="25" t="n">
+        <v>9.33918201E8</v>
+      </c>
+      <c r="X94" s="25" t="n">
+        <v>2.6203508E9</v>
+      </c>
+      <c r="Y94" s="25" t="n">
+        <v>1.1764989709E10</v>
+      </c>
+      <c r="Z94" s="25" t="n">
+        <v>4.444869849E9</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="26" t="s">
@@ -33362,6 +34374,18 @@
       <c r="V95" s="25" t="n">
         <v>1.33785258E8</v>
       </c>
+      <c r="W95" s="25" t="n">
+        <v>8.66154826E8</v>
+      </c>
+      <c r="X95" s="25" t="n">
+        <v>1.74716775E8</v>
+      </c>
+      <c r="Y95" s="25" t="n">
+        <v>9.97338928E8</v>
+      </c>
+      <c r="Z95" s="25" t="n">
+        <v>1.73665455E8</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="26" t="s">
@@ -33427,6 +34451,18 @@
       <c r="V96" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W96" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X96" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y96" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z96" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="26" t="s">
@@ -33492,6 +34528,18 @@
       <c r="V97" s="25" t="n">
         <v>6.558699518E9</v>
       </c>
+      <c r="W97" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X97" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y97" s="25" t="n">
+        <v>1.7544781846E10</v>
+      </c>
+      <c r="Z97" s="25" t="n">
+        <v>1.2264667528E10</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="26" t="s">
@@ -33557,6 +34605,18 @@
       <c r="V98" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W98" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X98" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y98" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z98" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="26" t="s">
@@ -33622,6 +34682,18 @@
       <c r="V99" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W99" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X99" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y99" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z99" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="28" t="s">
@@ -33687,6 +34759,18 @@
       <c r="V100" s="25" t="n">
         <v>1.0E7</v>
       </c>
+      <c r="W100" s="25" t="n">
+        <v>1.0E7</v>
+      </c>
+      <c r="X100" s="25" t="n">
+        <v>4.406336146E9</v>
+      </c>
+      <c r="Y100" s="25" t="n">
+        <v>1.0E7</v>
+      </c>
+      <c r="Z100" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="26" t="s">
@@ -33752,6 +34836,18 @@
       <c r="V101" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W101" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X101" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y101" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z101" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="26" t="s">
@@ -33817,6 +34913,18 @@
       <c r="V102" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W102" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X102" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y102" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z102" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="26" t="s">
@@ -33882,6 +34990,18 @@
       <c r="V103" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W103" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X103" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y103" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z103" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="26" t="s">
@@ -33947,6 +35067,18 @@
       <c r="V104" s="25" t="n">
         <v>1.0E7</v>
       </c>
+      <c r="W104" s="25" t="n">
+        <v>1.0E7</v>
+      </c>
+      <c r="X104" s="25" t="n">
+        <v>4.406336146E9</v>
+      </c>
+      <c r="Y104" s="25" t="n">
+        <v>1.0E7</v>
+      </c>
+      <c r="Z104" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="28" t="s">
@@ -34012,6 +35144,18 @@
       <c r="V105" s="25" t="n">
         <v>3.4979222091E10</v>
       </c>
+      <c r="W105" s="25" t="n">
+        <v>3.0182791842E10</v>
+      </c>
+      <c r="X105" s="25" t="n">
+        <v>4.5462005366E10</v>
+      </c>
+      <c r="Y105" s="25" t="n">
+        <v>2.492925508E10</v>
+      </c>
+      <c r="Z105" s="25" t="n">
+        <v>2.7508215534E10</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="26" t="s">
@@ -34077,6 +35221,18 @@
       <c r="V106" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W106" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X106" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y106" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z106" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="26" t="s">
@@ -34142,6 +35298,18 @@
       <c r="V107" s="25" t="n">
         <v>7.721E7</v>
       </c>
+      <c r="W107" s="25" t="n">
+        <v>2.597E7</v>
+      </c>
+      <c r="X107" s="25" t="n">
+        <v>1.08342E8</v>
+      </c>
+      <c r="Y107" s="25" t="n">
+        <v>2.8611E7</v>
+      </c>
+      <c r="Z107" s="25" t="n">
+        <v>3.48881E8</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="26" t="s">
@@ -34207,6 +35375,18 @@
       <c r="V108" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W108" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X108" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y108" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z108" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="26" t="s">
@@ -34272,6 +35452,18 @@
       <c r="V109" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W109" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X109" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y109" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z109" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="26" t="s">
@@ -34337,6 +35529,18 @@
       <c r="V110" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W110" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X110" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y110" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z110" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="26" t="s">
@@ -34402,6 +35606,18 @@
       <c r="V111" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W111" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X111" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y111" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z111" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="26" t="s">
@@ -34467,6 +35683,18 @@
       <c r="V112" s="25" t="n">
         <v>2.4959276218E10</v>
       </c>
+      <c r="W112" s="25" t="n">
+        <v>2.0633289631E10</v>
+      </c>
+      <c r="X112" s="25" t="n">
+        <v>2.0894894295E10</v>
+      </c>
+      <c r="Y112" s="25" t="n">
+        <v>1.5433450008E10</v>
+      </c>
+      <c r="Z112" s="25" t="n">
+        <v>1.7832575351E10</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="26" t="s">
@@ -34532,6 +35760,18 @@
       <c r="V113" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W113" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X113" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y113" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z113" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="26" t="s">
@@ -34597,6 +35837,18 @@
       <c r="V114" s="25" t="n">
         <v>9.942735873E9</v>
       </c>
+      <c r="W114" s="25" t="n">
+        <v>9.523532211E9</v>
+      </c>
+      <c r="X114" s="25" t="n">
+        <v>2.4458769071E10</v>
+      </c>
+      <c r="Y114" s="25" t="n">
+        <v>9.467194072E9</v>
+      </c>
+      <c r="Z114" s="25" t="n">
+        <v>9.326759183E9</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="28" t="s">
@@ -34662,6 +35914,18 @@
       <c r="V115" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W115" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X115" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y115" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z115" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="26" t="s">
@@ -34727,6 +35991,18 @@
       <c r="V116" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W116" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X116" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y116" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z116" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="26" t="s">
@@ -34792,6 +36068,18 @@
       <c r="V117" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W117" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X117" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y117" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z117" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="26" t="s">
@@ -34857,6 +36145,18 @@
       <c r="V118" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W118" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X118" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y118" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z118" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="26" t="s">
@@ -34922,6 +36222,18 @@
       <c r="V119" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W119" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X119" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y119" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z119" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="26" t="s">
@@ -34987,6 +36299,18 @@
       <c r="V120" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W120" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X120" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y120" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z120" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="28" t="s">
@@ -35052,6 +36376,18 @@
       <c r="V121" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W121" s="25" t="n">
+        <v>3.0E11</v>
+      </c>
+      <c r="X121" s="25" t="n">
+        <v>3.0E11</v>
+      </c>
+      <c r="Y121" s="25" t="n">
+        <v>3.0E11</v>
+      </c>
+      <c r="Z121" s="25" t="n">
+        <v>3.0E11</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="26" t="s">
@@ -35117,6 +36453,18 @@
       <c r="V122" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W122" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X122" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y122" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z122" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="26" t="s">
@@ -35182,6 +36530,18 @@
       <c r="V123" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W123" s="25" t="n">
+        <v>3.0E11</v>
+      </c>
+      <c r="X123" s="25" t="n">
+        <v>3.0E11</v>
+      </c>
+      <c r="Y123" s="25" t="n">
+        <v>3.0E11</v>
+      </c>
+      <c r="Z123" s="25" t="n">
+        <v>3.0E11</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="28" t="s">
@@ -35247,6 +36607,18 @@
       <c r="V124" s="25" t="n">
         <v>5.6017533428E10</v>
       </c>
+      <c r="W124" s="25" t="n">
+        <v>5.7183942942E10</v>
+      </c>
+      <c r="X124" s="25" t="n">
+        <v>5.7469346777E10</v>
+      </c>
+      <c r="Y124" s="25" t="n">
+        <v>7.3500576927E10</v>
+      </c>
+      <c r="Z124" s="25" t="n">
+        <v>5.730003306E10</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="26" t="s">
@@ -35312,6 +36684,18 @@
       <c r="V125" s="25" t="n">
         <v>5.48063974E8</v>
       </c>
+      <c r="W125" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X125" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y125" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z125" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="26" t="s">
@@ -35377,6 +36761,18 @@
       <c r="V126" s="25" t="n">
         <v>5.5469469454E10</v>
       </c>
+      <c r="W126" s="25" t="n">
+        <v>5.7183942942E10</v>
+      </c>
+      <c r="X126" s="25" t="n">
+        <v>5.7469346777E10</v>
+      </c>
+      <c r="Y126" s="25" t="n">
+        <v>7.3500576927E10</v>
+      </c>
+      <c r="Z126" s="25" t="n">
+        <v>5.730003306E10</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="26" t="s">
@@ -35442,6 +36838,18 @@
       <c r="V127" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W127" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X127" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y127" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z127" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="28" t="s">
@@ -35507,6 +36915,18 @@
       <c r="V128" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W128" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X128" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y128" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z128" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="26" t="s">
@@ -35572,6 +36992,18 @@
       <c r="V129" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W129" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X129" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y129" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z129" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="26" t="s">
@@ -35637,6 +37069,18 @@
       <c r="V130" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W130" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X130" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y130" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z130" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="26" t="s">
@@ -35702,6 +37146,18 @@
       <c r="V131" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W131" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X131" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y131" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z131" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="26" t="s">
@@ -35767,6 +37223,18 @@
       <c r="V132" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W132" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X132" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y132" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z132" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="26" t="s">
@@ -35832,6 +37300,18 @@
       <c r="V133" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W133" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X133" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y133" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z133" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="26" t="s">
@@ -35897,6 +37377,18 @@
       <c r="V134" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W134" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X134" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y134" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z134" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="28" t="s">
@@ -35962,6 +37454,18 @@
       <c r="V135" s="25" t="n">
         <v>1.6082544001E10</v>
       </c>
+      <c r="W135" s="25" t="n">
+        <v>1.4709690203E10</v>
+      </c>
+      <c r="X135" s="25" t="n">
+        <v>1.4434339331E10</v>
+      </c>
+      <c r="Y135" s="25" t="n">
+        <v>1.6609969787E10</v>
+      </c>
+      <c r="Z135" s="25" t="n">
+        <v>8.982355039E9</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="26" t="s">
@@ -36027,6 +37531,18 @@
       <c r="V136" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W136" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X136" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y136" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z136" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="26" t="s">
@@ -36092,6 +37608,18 @@
       <c r="V137" s="25" t="n">
         <v>1.093518518E9</v>
       </c>
+      <c r="W137" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X137" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y137" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z137" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="26" t="s">
@@ -36157,6 +37685,18 @@
       <c r="V138" s="25" t="n">
         <v>1.4989025483E10</v>
       </c>
+      <c r="W138" s="25" t="n">
+        <v>1.4709690203E10</v>
+      </c>
+      <c r="X138" s="25" t="n">
+        <v>1.4434339331E10</v>
+      </c>
+      <c r="Y138" s="25" t="n">
+        <v>1.6609969787E10</v>
+      </c>
+      <c r="Z138" s="25" t="n">
+        <v>8.982355039E9</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" s="26" t="s">
@@ -36222,6 +37762,18 @@
       <c r="V139" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W139" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X139" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y139" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z139" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="26" t="s">
@@ -36287,6 +37839,18 @@
       <c r="V140" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W140" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X140" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y140" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z140" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="26" t="s">
@@ -36352,6 +37916,18 @@
       <c r="V141" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W141" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X141" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y141" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z141" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="26" t="s">
@@ -36417,6 +37993,18 @@
       <c r="V142" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W142" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X142" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y142" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z142" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" s="26" t="s">
@@ -36482,6 +38070,18 @@
       <c r="V143" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W143" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X143" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y143" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z143" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="28" t="s">
@@ -36547,6 +38147,18 @@
       <c r="V144" s="25" t="n">
         <v>1.033822654E10</v>
       </c>
+      <c r="W144" s="25" t="n">
+        <v>8.167292229E9</v>
+      </c>
+      <c r="X144" s="25" t="n">
+        <v>1.0161677606E10</v>
+      </c>
+      <c r="Y144" s="25" t="n">
+        <v>7.867516939E9</v>
+      </c>
+      <c r="Z144" s="25" t="n">
+        <v>1.1814328629E10</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="26" t="s">
@@ -36612,6 +38224,18 @@
       <c r="V145" s="25" t="n">
         <v>8.82902654E9</v>
       </c>
+      <c r="W145" s="25" t="n">
+        <v>6.68702187E8</v>
+      </c>
+      <c r="X145" s="25" t="n">
+        <v>6.386160324E9</v>
+      </c>
+      <c r="Y145" s="25" t="n">
+        <v>1.510133824E9</v>
+      </c>
+      <c r="Z145" s="25" t="n">
+        <v>8.315895864E9</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="26" t="s">
@@ -36677,6 +38301,18 @@
       <c r="V146" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W146" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X146" s="25" t="n">
+        <v>3.310657542E9</v>
+      </c>
+      <c r="Y146" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z146" s="25" t="n">
+        <v>1.436502046E9</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="26" t="s">
@@ -36742,6 +38378,18 @@
       <c r="V147" s="25" t="n">
         <v>1.5092E9</v>
       </c>
+      <c r="W147" s="25" t="n">
+        <v>7.0120375E9</v>
+      </c>
+      <c r="X147" s="25" t="n">
+        <v>3.5E8</v>
+      </c>
+      <c r="Y147" s="25" t="n">
+        <v>6.3331175E9</v>
+      </c>
+      <c r="Z147" s="25" t="n">
+        <v>6.9552E8</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="26" t="s">
@@ -36807,6 +38455,18 @@
       <c r="V148" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W148" s="25" t="n">
+        <v>7.2172092E7</v>
+      </c>
+      <c r="X148" s="25" t="n">
+        <v>1.04737674E8</v>
+      </c>
+      <c r="Y148" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z148" s="25" t="n">
+        <v>1.023510914E9</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="26" t="s">
@@ -36872,6 +38532,18 @@
       <c r="V149" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W149" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X149" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y149" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z149" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" s="26" t="s">
@@ -36937,6 +38609,18 @@
       <c r="V150" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W150" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X150" s="25" t="n">
+        <v>183456.0</v>
+      </c>
+      <c r="Y150" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z150" s="25" t="n">
+        <v>298533.0</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" s="26" t="s">
@@ -37002,6 +38686,18 @@
       <c r="V151" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W151" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X151" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y151" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z151" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" s="26" t="s">
@@ -37067,6 +38763,18 @@
       <c r="V152" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W152" s="25" t="n">
+        <v>4.1438045E8</v>
+      </c>
+      <c r="X152" s="25" t="n">
+        <v>-4.1438045E8</v>
+      </c>
+      <c r="Y152" s="25" t="n">
+        <v>2.4265615E7</v>
+      </c>
+      <c r="Z152" s="25" t="n">
+        <v>7.66920332E8</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" s="26" t="s">
@@ -37132,6 +38840,18 @@
       <c r="V153" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W153" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X153" s="25" t="n">
+        <v>4.2431906E8</v>
+      </c>
+      <c r="Y153" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z153" s="25" t="n">
+        <v>-4.2431906E8</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" s="28" t="s">
@@ -37197,6 +38917,18 @@
       <c r="V154" s="25" t="n">
         <v>-5.68786587E8</v>
       </c>
+      <c r="W154" s="25" t="n">
+        <v>-3.3374233E7</v>
+      </c>
+      <c r="X154" s="25" t="n">
+        <v>2.427371643E9</v>
+      </c>
+      <c r="Y154" s="25" t="n">
+        <v>139321.0</v>
+      </c>
+      <c r="Z154" s="25" t="n">
+        <v>1.1456521499E10</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" s="26" t="s">
@@ -37262,6 +38994,18 @@
       <c r="V155" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W155" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X155" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y155" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z155" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" s="26" t="s">
@@ -37327,6 +39071,18 @@
       <c r="V156" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W156" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X156" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y156" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z156" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" s="26" t="s">
@@ -37392,6 +39148,18 @@
       <c r="V157" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W157" s="25" t="n">
+        <v>3300000.0</v>
+      </c>
+      <c r="X157" s="25" t="n">
+        <v>-3300000.0</v>
+      </c>
+      <c r="Y157" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z157" s="25" t="n">
+        <v>2.1036169325E10</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" s="26" t="s">
@@ -37457,6 +39225,18 @@
       <c r="V158" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W158" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X158" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y158" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z158" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" s="26" t="s">
@@ -37522,6 +39302,18 @@
       <c r="V159" s="25" t="n">
         <v>70380.0</v>
       </c>
+      <c r="W159" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X159" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y159" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z159" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" s="26" t="s">
@@ -37587,6 +39379,18 @@
       <c r="V160" s="25" t="n">
         <v>0.0</v>
       </c>
+      <c r="W160" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X160" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y160" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z160" s="25" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" s="26" t="s">
@@ -37652,6 +39456,18 @@
       <c r="V161" s="25" t="n">
         <v>-5.69081501E8</v>
       </c>
+      <c r="W161" s="25" t="n">
+        <v>-3.6924975E7</v>
+      </c>
+      <c r="X161" s="25" t="n">
+        <v>2.424719583E9</v>
+      </c>
+      <c r="Y161" s="25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z161" s="25" t="n">
+        <v>-9.573936626E9</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" s="26" t="s">
@@ -37717,6 +39533,18 @@
       <c r="V162" s="25" t="n">
         <v>224534.0</v>
       </c>
+      <c r="W162" s="25" t="n">
+        <v>250742.0</v>
+      </c>
+      <c r="X162" s="25" t="n">
+        <v>5952060.0</v>
+      </c>
+      <c r="Y162" s="25" t="n">
+        <v>139321.0</v>
+      </c>
+      <c r="Z162" s="25" t="n">
+        <v>-5711200.0</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" s="28" t="s">
@@ -37782,6 +39610,18 @@
       <c r="V163" s="25" t="n">
         <v>1.5358230472E10</v>
       </c>
+      <c r="W163" s="25" t="n">
+        <v>1.8935253288E10</v>
+      </c>
+      <c r="X163" s="25" t="n">
+        <v>1.6826197606E10</v>
+      </c>
+      <c r="Y163" s="25" t="n">
+        <v>1.6557190422E10</v>
+      </c>
+      <c r="Z163" s="25" t="n">
+        <v>5.7046852173E10</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" s="26" t="s">
@@ -37847,6 +39687,18 @@
       <c r="V164" s="25" t="n">
         <v>1.35099507E8</v>
       </c>
+      <c r="W164" s="25" t="n">
+        <v>1.84946153E8</v>
+      </c>
+      <c r="X164" s="25" t="n">
+        <v>1.61543692E8</v>
+      </c>
+      <c r="Y164" s="25" t="n">
+        <v>1.77598776E8</v>
+      </c>
+      <c r="Z164" s="25" t="n">
+        <v>1.56577456E8</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" s="26" t="s">
@@ -37912,6 +39764,18 @@
       <c r="V165" s="25" t="n">
         <v>6.523828564E9</v>
       </c>
+      <c r="W165" s="25" t="n">
+        <v>6.570313503E9</v>
+      </c>
+      <c r="X165" s="25" t="n">
+        <v>6.830567114E9</v>
+      </c>
+      <c r="Y165" s="25" t="n">
+        <v>5.790457003E9</v>
+      </c>
+      <c r="Z165" s="25" t="n">
+        <v>7.511147044E9</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" s="26" t="s">
@@ -37977,6 +39841,18 @@
       <c r="V166" s="25" t="n">
         <v>1.65186459E8</v>
       </c>
+      <c r="W166" s="25" t="n">
+        <v>1.593723911E9</v>
+      </c>
+      <c r="X166" s="25" t="n">
+        <v>1.596394755E9</v>
+      </c>
+      <c r="Y166" s="25" t="n">
+        <v>1.639244485E9</v>
+      </c>
+      <c r="Z166" s="25" t="n">
+        <v>3.915178749E10</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" s="26" t="s">
@@ -38042,6 +39918,18 @@
       <c r="V167" s="25" t="n">
         <v>7.44432906E9</v>
       </c>
+      <c r="W167" s="25" t="n">
+        <v>9.004177118E9</v>
+      </c>
+      <c r="X167" s="25" t="n">
+        <v>7.329117564E9</v>
+      </c>
+      <c r="Y167" s="25" t="n">
+        <v>7.404103657E9</v>
+      </c>
+      <c r="Z167" s="25" t="n">
+        <v>9.694934966E9</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" s="26" t="s">
@@ -38106,6 +39994,18 @@
       </c>
       <c r="V168" s="25" t="n">
         <v>1.089786882E9</v>
+      </c>
+      <c r="W168" s="25" t="n">
+        <v>1.582092603E9</v>
+      </c>
+      <c r="X168" s="25" t="n">
+        <v>9.08574481E8</v>
+      </c>
+      <c r="Y168" s="25" t="n">
+        <v>1.545786501E9</v>
+      </c>
+      <c r="Z168" s="25" t="n">
+        <v>5.32405217E8</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
@@ -38146,7 +40046,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="E10:V10"/>
+    <mergeCell ref="E10:Z10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A174" r:id="rId1" display="https://www.vietcap.com.vn/" xr:uid="{D6386FB0-752A-884E-829A-45A876D98EB2}"/>

</xml_diff>